<commit_message>
Update IP - EX 10 - Funcoes e formulas do excel II (Anexo).xlsx
</commit_message>
<xml_diff>
--- a/Materia_2-PowerBi/IP - EX 10 - Funcoes e formulas do excel II (Anexo).xlsx
+++ b/Materia_2-PowerBi/IP - EX 10 - Funcoes e formulas do excel II (Anexo).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bianc\4)DNC\Repositorio\DNC_DataScience\Materia_2-PowerBi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EB254905-7007-4F56-94CE-85ABA9FF6E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78823258-69E4-4A30-892A-2CE5D28D16B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CONTEÚDO" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="EXERCICIO 1" sheetId="15" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'EXERCICIO 1'!$B$2:$C$399</definedName>
     <definedName name="anscount" hidden="1">2</definedName>
     <definedName name="Bancos">#REF!</definedName>
     <definedName name="conta">#REF!</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="76">
   <si>
     <t>OUTRAS INFORMAÇÕES</t>
   </si>
@@ -246,13 +247,35 @@
   </si>
   <si>
     <t>casa</t>
+  </si>
+  <si>
+    <t>Lorenzo</t>
+  </si>
+  <si>
+    <t>Bianchi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">, </t>
+  </si>
+  <si>
+    <t>Bianca</t>
+  </si>
+  <si>
+    <t>Maya</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> e </t>
+  </si>
+  <si>
+    <t>SOMA DE VALORES MAIORES QUE 10 REAIS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
@@ -931,7 +954,7 @@
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1077,6 +1100,9 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="4" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1335,7 +1361,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
+      <xdr:colOff>923925</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
@@ -1352,8 +1378,64 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4657725" y="1752600"/>
-          <a:ext cx="390525" cy="0"/>
+          <a:off x="4819650" y="1752600"/>
+          <a:ext cx="771525" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="002060"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>923925</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="2" name="Conector de Seta Reta 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BA82636-2056-4E81-A931-F96124561DE1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4953000" y="1943100"/>
+          <a:ext cx="638175" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1674,7 +1756,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:R22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
@@ -1960,7 +2042,7 @@
   <dimension ref="B2:Q192"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="O32" sqref="O32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2134,9 +2216,18 @@
       </c>
     </row>
     <row r="15" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="F15" s="25"/>
+      <c r="B15" s="25">
+        <f>COUNT(B9:B14)</f>
+        <v>5</v>
+      </c>
+      <c r="D15" s="25">
+        <f>COUNTA(D9:D14)</f>
+        <v>4</v>
+      </c>
+      <c r="F15" s="25">
+        <f>COUNTBLANK(F9:F14)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="2:17" s="21" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B16" s="21" t="s">
@@ -2155,7 +2246,10 @@
       </c>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="64"/>
+      <c r="B19" s="64">
+        <f>LEN(B18)</f>
+        <v>4</v>
+      </c>
       <c r="C19" s="65"/>
       <c r="D19" s="66"/>
     </row>
@@ -2163,47 +2257,143 @@
       <c r="B20" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="H20" s="27"/>
-      <c r="I20" s="27"/>
-      <c r="J20" s="27"/>
-      <c r="K20" s="27"/>
-      <c r="M20" s="27"/>
-      <c r="N20" s="27"/>
-      <c r="O20" s="27"/>
-      <c r="P20" s="27"/>
+      <c r="H20" s="27">
+        <f ca="1">RAND()</f>
+        <v>1.0181750581898186E-2</v>
+      </c>
+      <c r="I20" s="70">
+        <f ca="1">RANDBETWEEN(1,100)</f>
+        <v>71</v>
+      </c>
+      <c r="J20" s="69">
+        <f ca="1">RANDBETWEEN(1,100)/10</f>
+        <v>6.7</v>
+      </c>
+      <c r="K20" s="69">
+        <f ca="1">RANDBETWEEN(10,100)/10</f>
+        <v>5.2</v>
+      </c>
+      <c r="M20" s="27">
+        <f ca="1">ROUND(H20,0)</f>
+        <v>0</v>
+      </c>
+      <c r="N20" s="27">
+        <f t="shared" ref="N20:P25" ca="1" si="0">ROUND(I20,0)</f>
+        <v>71</v>
+      </c>
+      <c r="O20" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="P20" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="H21" s="27"/>
-      <c r="I21" s="27"/>
-      <c r="J21" s="27"/>
-      <c r="K21" s="27"/>
-      <c r="M21" s="27"/>
-      <c r="N21" s="27"/>
-      <c r="O21" s="27"/>
-      <c r="P21" s="27"/>
+      <c r="H21" s="27">
+        <f t="shared" ref="H21:H25" ca="1" si="1">RAND()</f>
+        <v>0.35551248545913494</v>
+      </c>
+      <c r="I21" s="70">
+        <f t="shared" ref="I21:K25" ca="1" si="2">RANDBETWEEN(1,100)</f>
+        <v>62</v>
+      </c>
+      <c r="J21" s="69">
+        <f t="shared" ref="J21:J25" ca="1" si="3">RANDBETWEEN(1,100)/10</f>
+        <v>2.5</v>
+      </c>
+      <c r="K21" s="69">
+        <f t="shared" ref="K21:K25" ca="1" si="4">RANDBETWEEN(10,100)/10</f>
+        <v>3.8</v>
+      </c>
+      <c r="M21" s="27">
+        <f t="shared" ref="M21:M25" ca="1" si="5">ROUND(H21,0)</f>
+        <v>0</v>
+      </c>
+      <c r="N21" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="O21" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="P21" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B22" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="H22" s="27"/>
-      <c r="I22" s="27"/>
-      <c r="J22" s="27"/>
-      <c r="K22" s="27"/>
-      <c r="M22" s="27"/>
-      <c r="N22" s="27"/>
-      <c r="O22" s="27"/>
-      <c r="P22" s="27"/>
+      <c r="H22" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.30532179593492781</v>
+      </c>
+      <c r="I22" s="70">
+        <f t="shared" ca="1" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="J22" s="69">
+        <f t="shared" ca="1" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="K22" s="69">
+        <f t="shared" ca="1" si="4"/>
+        <v>8.5</v>
+      </c>
+      <c r="M22" s="27">
+        <f t="shared" ca="1" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="N22" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="O22" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="P22" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="H23" s="27"/>
-      <c r="I23" s="27"/>
-      <c r="J23" s="27"/>
-      <c r="K23" s="27"/>
-      <c r="M23" s="27"/>
-      <c r="N23" s="27"/>
-      <c r="O23" s="27"/>
-      <c r="P23" s="27"/>
+      <c r="H23" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.55957501658511977</v>
+      </c>
+      <c r="I23" s="70">
+        <f t="shared" ca="1" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="J23" s="69">
+        <f t="shared" ca="1" si="3"/>
+        <v>2.6</v>
+      </c>
+      <c r="K23" s="69">
+        <f t="shared" ca="1" si="4"/>
+        <v>1.2</v>
+      </c>
+      <c r="M23" s="27">
+        <f t="shared" ca="1" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="N23" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="O23" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="P23" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
@@ -2212,30 +2402,83 @@
       <c r="D24" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="H24" s="27"/>
-      <c r="I24" s="27"/>
-      <c r="J24" s="27"/>
-      <c r="K24" s="27"/>
-      <c r="M24" s="27"/>
-      <c r="N24" s="27"/>
-      <c r="O24" s="27"/>
-      <c r="P24" s="27"/>
+      <c r="H24" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.91779302345113967</v>
+      </c>
+      <c r="I24" s="70">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="J24" s="69">
+        <f t="shared" ca="1" si="3"/>
+        <v>5.4</v>
+      </c>
+      <c r="K24" s="69">
+        <f t="shared" ca="1" si="4"/>
+        <v>6.8</v>
+      </c>
+      <c r="M24" s="27">
+        <f t="shared" ca="1" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="N24" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="O24" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="P24" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="25" spans="2:16" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="20"/>
+      <c r="B25" s="20" t="s">
+        <v>69</v>
+      </c>
       <c r="C25"/>
-      <c r="D25" s="64"/>
+      <c r="D25" s="64" t="str">
+        <f>_xlfn.CONCAT(B25,"e ",B28)</f>
+        <v>Lorenzoe Bianchi</v>
+      </c>
       <c r="E25" s="65"/>
       <c r="F25" s="66"/>
-      <c r="H25" s="27"/>
-      <c r="I25" s="27"/>
-      <c r="J25" s="27"/>
-      <c r="K25" s="27"/>
+      <c r="H25" s="27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.74618875873622914</v>
+      </c>
+      <c r="I25" s="70">
+        <f t="shared" ca="1" si="2"/>
+        <v>78</v>
+      </c>
+      <c r="J25" s="69">
+        <f t="shared" ca="1" si="3"/>
+        <v>5.6</v>
+      </c>
+      <c r="K25" s="69">
+        <f t="shared" ca="1" si="4"/>
+        <v>1.8</v>
+      </c>
       <c r="L25"/>
-      <c r="M25" s="27"/>
-      <c r="N25" s="27"/>
-      <c r="O25" s="27"/>
-      <c r="P25" s="27"/>
+      <c r="M25" s="27">
+        <f t="shared" ca="1" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="N25" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>78</v>
+      </c>
+      <c r="O25" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="P25" s="27">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.25">
       <c r="H26" s="21" t="s">
@@ -2264,8 +2507,13 @@
       </c>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B28" s="20"/>
-      <c r="D28" s="64"/>
+      <c r="B28" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="D28" s="64" t="str">
+        <f>B25&amp; "e "&amp;B28</f>
+        <v>Lorenzoe Bianchi</v>
+      </c>
       <c r="E28" s="65"/>
       <c r="F28" s="66"/>
       <c r="H28" s="28" t="s">
@@ -2283,19 +2531,59 @@
       <c r="I31" s="2"/>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D32" s="64"/>
+      <c r="B32" t="s">
+        <v>69</v>
+      </c>
+      <c r="D32" s="64" t="str">
+        <f>_xlfn.CONCAT(B32:B36)</f>
+        <v>Lorenzo, Bianca e Maya</v>
+      </c>
       <c r="E32" s="65"/>
       <c r="F32" s="66"/>
     </row>
-    <row r="34" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>72</v>
+      </c>
       <c r="D34" s="26" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="35" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D35" s="64"/>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>74</v>
+      </c>
+      <c r="D35" s="64" t="str">
+        <f>_xlfn.TEXTJOIN("-",TRUE,B38:B42)</f>
+        <v>Lorenzo-Bianca-Maya</v>
+      </c>
       <c r="E35" s="65"/>
       <c r="F35" s="66"/>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="192" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C192" s="61" t="s">
@@ -2334,16 +2622,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:J399"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
     <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.85546875" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2368,7 +2657,10 @@
       <c r="E3" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="16"/>
+      <c r="F3" s="16">
+        <f>MIN($C$3:$C$399)</f>
+        <v>3.48</v>
+      </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="29" t="s">
@@ -2380,7 +2672,10 @@
       <c r="E4" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="16"/>
+      <c r="F4" s="16">
+        <f>MAX($C$3:$C$399)</f>
+        <v>14.9</v>
+      </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="29" t="s">
@@ -2392,7 +2687,10 @@
       <c r="E5" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="16"/>
+      <c r="F5" s="16">
+        <f>AVERAGE($C$3:$C$399)</f>
+        <v>8.9564483627203959</v>
+      </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="29" t="s">
@@ -2404,7 +2702,10 @@
       <c r="E6" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="16"/>
+      <c r="F6" s="16">
+        <f>MEDIAN($C$3:$C$399)</f>
+        <v>8.84</v>
+      </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="29" t="s">
@@ -2416,13 +2717,19 @@
       <c r="E7" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="16"/>
+      <c r="F7" s="16">
+        <f>SUM(C3:C399)</f>
+        <v>3555.7099999999973</v>
+      </c>
       <c r="G7" s="67" t="s">
         <v>60</v>
       </c>
       <c r="H7" s="67"/>
       <c r="I7" s="68"/>
-      <c r="J7" s="16"/>
+      <c r="J7" s="16">
+        <f>COUNT(C3:C399)</f>
+        <v>397</v>
+      </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="29" t="s">
@@ -2456,47 +2763,49 @@
       <c r="F10" s="38"/>
       <c r="G10" s="38"/>
       <c r="H10" s="39"/>
-      <c r="I10" s="16"/>
-    </row>
-    <row r="11" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I10" s="71">
+        <f>F7*0.15</f>
+        <v>533.35649999999953</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="29" t="s">
         <v>24</v>
       </c>
       <c r="C11" s="30">
         <v>10.98</v>
       </c>
-    </row>
-    <row r="12" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E11" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="I11" s="71">
+        <f>SUMIF($C$3:$C$399,"&gt;10")</f>
+        <v>2050.7199999999989</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="29" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="30">
         <v>9.6199999999999992</v>
       </c>
-      <c r="E12" s="41" t="s">
-        <v>54</v>
-      </c>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
-      <c r="J12" s="43"/>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B13" s="29" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="30">
         <v>12.65</v>
       </c>
-      <c r="E13" s="47" t="s">
-        <v>44</v>
-      </c>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="44"/>
+      <c r="E13" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="43"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="29" t="s">
@@ -2505,14 +2814,14 @@
       <c r="C14" s="30">
         <v>9.99</v>
       </c>
-      <c r="E14" s="48" t="s">
-        <v>45</v>
-      </c>
-      <c r="F14" s="45"/>
-      <c r="G14" s="45"/>
-      <c r="H14" s="45"/>
-      <c r="I14" s="45"/>
-      <c r="J14" s="46"/>
+      <c r="E14" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="44"/>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="29" t="s">
@@ -2521,6 +2830,14 @@
       <c r="C15" s="30">
         <v>7.69</v>
       </c>
+      <c r="E15" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="45"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="45"/>
+      <c r="J15" s="46"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="29" t="s">
@@ -5595,6 +5912,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="B2:C399" xr:uid="{00000000-0001-0000-0200-000000000000}"/>
   <mergeCells count="1">
     <mergeCell ref="G7:I7"/>
   </mergeCells>

</xml_diff>